<commit_message>
Cambios finales para la Actividad 1
</commit_message>
<xml_diff>
--- a/files/exp1_ruleta_1corte_epsilon.xlsx
+++ b/files/exp1_ruleta_1corte_epsilon.xlsx
@@ -10,7 +10,8 @@
     <sheet name="gen_0" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="gen_1" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="gen_2" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Función objetivo" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="gen_3" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Función objetivo" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -490,54 +491,54 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-1</v>
+        <v>-0.9682539682539683</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>000000</t>
+          <t>000001</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0.9375157470395565</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>110111</t>
+          <t>001100</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['110111' '110111']</t>
+          <t>['110100' '001000']</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>0.746031746031746</v>
+        <v>-0.6190476190476191</v>
       </c>
       <c r="J2" t="n">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>110111</t>
+          <t>001100</t>
         </is>
       </c>
       <c r="L2" t="n">
-        <v>0.5565633660871756</v>
+        <v>0.3832199546485261</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.746031746031746</v>
+        <v>-0.746031746031746</v>
       </c>
       <c r="B3" t="n">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>110111</t>
+          <t>001000</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -545,347 +546,347 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>110111</t>
+          <t>110000</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['110111' '110111']</t>
+          <t>['110100' '001000']</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>0.746031746031746</v>
+        <v>0.5238095238095237</v>
       </c>
       <c r="J3" t="n">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>110111</t>
+          <t>110000</t>
         </is>
       </c>
       <c r="L3" t="n">
-        <v>0.5565633660871756</v>
+        <v>0.27437641723356</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.7142857142857142</v>
+        <v>-0.7142857142857143</v>
       </c>
       <c r="B4" t="n">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>110110</t>
+          <t>001001</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.510204081632653</v>
+        <v>0.5102040816326531</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>110000</t>
+          <t>001110</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['000000' '110001']</t>
+          <t>['110110' '001000']</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>0.5238095238095237</v>
+        <v>-0.5555555555555556</v>
       </c>
       <c r="J4" t="n">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>110000</t>
+          <t>001110</t>
         </is>
       </c>
       <c r="L4" t="n">
-        <v>0.27437641723356</v>
+        <v>0.308641975308642</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.6190476190476191</v>
+        <v>0.7142857142857142</v>
       </c>
       <c r="B5" t="n">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>110011</t>
+          <t>110110</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.3832199546485261</v>
+        <v>0.510204081632653</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>000001</t>
+          <t>110000</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['000000' '110001']</t>
+          <t>['110110' '001000']</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>-0.9682539682539683</v>
+        <v>0.5238095238095237</v>
       </c>
       <c r="J5" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>000001</t>
+          <t>110000</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>0.9375157470395565</v>
+        <v>0.27437641723356</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
+        <v>0.6507936507936507</v>
+      </c>
+      <c r="B6" t="n">
+        <v>52</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>110100</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.4235323759133282</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>110001</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>['000001' '110100']</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
         <v>0.5555555555555554</v>
       </c>
-      <c r="B6" t="n">
+      <c r="J6" t="n">
         <v>49</v>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>110001</t>
         </is>
       </c>
-      <c r="D6" t="n">
+      <c r="L6" t="n">
         <v>0.3086419753086417</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>000000</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>['000000' '000000']</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>-1</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>000000</t>
-        </is>
-      </c>
-      <c r="L6" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.4603174603174602</v>
+        <v>0.5238095238095237</v>
       </c>
       <c r="B7" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>101110</t>
+          <t>110000</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.2118921642731166</v>
+        <v>0.27437641723356</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>000000</t>
+          <t>000100</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['000000' '000000']</t>
+          <t>['000001' '110100']</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>-1</v>
+        <v>-0.873015873015873</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>000000</t>
+          <t>000100</t>
         </is>
       </c>
       <c r="L7" t="n">
-        <v>1</v>
+        <v>0.762156714537667</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.4285714285714284</v>
+        <v>-0.3650793650793651</v>
       </c>
       <c r="B8" t="n">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>101101</t>
+          <t>010100</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.1836734693877549</v>
+        <v>0.1332829428067523</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>000001</t>
+          <t>001000</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['110001' '000000']</t>
+          <t>['001000' '001001']</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>-0.9682539682539683</v>
+        <v>-0.746031746031746</v>
       </c>
       <c r="J8" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>000001</t>
+          <t>001000</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>0.9375157470395565</v>
+        <v>0.5565633660871756</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.3968253968253967</v>
+        <v>0.2698412698412698</v>
       </c>
       <c r="B9" t="n">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>101100</t>
+          <t>101000</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.1574703955656336</v>
+        <v>0.07281431090954897</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>110000</t>
+          <t>001001</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['110001' '000000']</t>
+          <t>['001000' '001001']</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>0.5238095238095237</v>
+        <v>-0.7142857142857143</v>
       </c>
       <c r="J9" t="n">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>110000</t>
+          <t>001001</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>0.27437641723356</v>
+        <v>0.5102040816326531</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-0.3015873015873016</v>
+        <v>0.2063492063492063</v>
       </c>
       <c r="B10" t="n">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>010110</t>
+          <t>100110</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.09095490047871002</v>
+        <v>0.04257999496094732</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>110110</t>
+          <t>001001</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['010110' '110001']</t>
+          <t>['001001' '001001']</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>0.7142857142857142</v>
+        <v>-0.7142857142857143</v>
       </c>
       <c r="J10" t="n">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>110110</t>
+          <t>001001</t>
         </is>
       </c>
       <c r="L10" t="n">
-        <v>0.510204081632653</v>
+        <v>0.5102040816326531</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>-0.2380952380952381</v>
+        <v>0.1746031746031744</v>
       </c>
       <c r="B11" t="n">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>011000</t>
+          <t>100101</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.05668934240362813</v>
+        <v>0.03048626858150661</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>010001</t>
+          <t>001001</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['010110' '110001']</t>
+          <t>['001001' '001001']</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>-0.4603174603174603</v>
+        <v>-0.7142857142857143</v>
       </c>
       <c r="J11" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>010001</t>
+          <t>001001</t>
         </is>
       </c>
       <c r="L11" t="n">
-        <v>0.2118921642731167</v>
+        <v>0.5102040816326531</v>
       </c>
     </row>
   </sheetData>
@@ -961,322 +962,322 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-1</v>
+        <v>-0.9682539682539683</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>000000</t>
+          <t>000001</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0.9375157470395565</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>110001</t>
+          <t>001000</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['000001' '110111']</t>
+          <t>['001000' '001000']</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>0.5555555555555554</v>
+        <v>-0.746031746031746</v>
       </c>
       <c r="J2" t="n">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>110001</t>
+          <t>001000</t>
         </is>
       </c>
       <c r="L2" t="n">
-        <v>0.3086419753086417</v>
+        <v>0.5565633660871756</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-1</v>
+        <v>-0.873015873015873</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>000000</t>
+          <t>000100</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0.762156714537667</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>000111</t>
+          <t>001000</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['000001' '110111']</t>
+          <t>['001000' '001000']</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>-0.7777777777777778</v>
+        <v>-0.746031746031746</v>
       </c>
       <c r="J3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>000111</t>
+          <t>001000</t>
         </is>
       </c>
       <c r="L3" t="n">
-        <v>0.6049382716049383</v>
+        <v>0.5565633660871756</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-1</v>
+        <v>-0.746031746031746</v>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>000000</t>
+          <t>001000</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0.5565633660871756</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>110110</t>
+          <t>110000</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['110110' '110111']</t>
+          <t>['001000' '110110']</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>0.7142857142857142</v>
+        <v>0.5238095238095237</v>
       </c>
       <c r="J4" t="n">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>110110</t>
+          <t>110000</t>
         </is>
       </c>
       <c r="L4" t="n">
-        <v>0.510204081632653</v>
+        <v>0.27437641723356</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-0.9682539682539683</v>
+        <v>-0.746031746031746</v>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>000001</t>
+          <t>001000</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.9375157470395565</v>
+        <v>0.5565633660871756</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>110111</t>
+          <t>001110</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['110110' '110111']</t>
+          <t>['001000' '110110']</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0.746031746031746</v>
+        <v>-0.5555555555555556</v>
       </c>
       <c r="J5" t="n">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>110111</t>
+          <t>001110</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>0.5565633660871756</v>
+        <v>0.308641975308642</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.9682539682539683</v>
+        <v>-0.7142857142857143</v>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>000001</t>
+          <t>001001</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.9375157470395565</v>
+        <v>0.5102040816326531</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>110001</t>
+          <t>000110</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['000001' '110111']</t>
+          <t>['110110' '000100']</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>0.5555555555555554</v>
+        <v>-0.8095238095238095</v>
       </c>
       <c r="J6" t="n">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>110001</t>
+          <t>000110</t>
         </is>
       </c>
       <c r="L6" t="n">
-        <v>0.3086419753086417</v>
+        <v>0.655328798185941</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.746031746031746</v>
+        <v>-0.7142857142857143</v>
       </c>
       <c r="B7" t="n">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>110111</t>
+          <t>001001</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.5565633660871756</v>
+        <v>0.5102040816326531</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>000111</t>
+          <t>110100</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['000001' '110111']</t>
+          <t>['110110' '000100']</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>-0.7777777777777778</v>
+        <v>0.6507936507936507</v>
       </c>
       <c r="J7" t="n">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>000111</t>
+          <t>110100</t>
         </is>
       </c>
       <c r="L7" t="n">
-        <v>0.6049382716049383</v>
+        <v>0.4235323759133282</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.746031746031746</v>
+        <v>-0.7142857142857143</v>
       </c>
       <c r="B8" t="n">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>110111</t>
+          <t>001001</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.5565633660871756</v>
+        <v>0.5102040816326531</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>110000</t>
+          <t>001001</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['000000' '110110']</t>
+          <t>['001001' '001000']</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>0.5238095238095237</v>
+        <v>-0.7142857142857143</v>
       </c>
       <c r="J8" t="n">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>110000</t>
+          <t>001001</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>0.27437641723356</v>
+        <v>0.5102040816326531</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.746031746031746</v>
+        <v>-0.7142857142857143</v>
       </c>
       <c r="B9" t="n">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>110111</t>
+          <t>001001</t>
         </is>
       </c>
       <c r="D9" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>001000</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>['001001' '001000']</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>-0.746031746031746</v>
+      </c>
+      <c r="J9" t="n">
+        <v>8</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>001000</t>
+        </is>
+      </c>
+      <c r="L9" t="n">
         <v>0.5565633660871756</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>000110</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>['000000' '110110']</t>
-        </is>
-      </c>
-      <c r="I9" t="n">
-        <v>-0.8095238095238095</v>
-      </c>
-      <c r="J9" t="n">
-        <v>6</v>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>000110</t>
-        </is>
-      </c>
-      <c r="L9" t="n">
-        <v>0.655328798185941</v>
       </c>
     </row>
     <row r="10">
@@ -1296,67 +1297,67 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>110000</t>
+          <t>001110</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['000000' '110111']</t>
+          <t>['110110' '001000']</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>0.5238095238095237</v>
+        <v>-0.5555555555555556</v>
       </c>
       <c r="J10" t="n">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>110000</t>
+          <t>001110</t>
         </is>
       </c>
       <c r="L10" t="n">
-        <v>0.27437641723356</v>
+        <v>0.308641975308642</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.7142857142857142</v>
+        <v>0.6507936507936507</v>
       </c>
       <c r="B11" t="n">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>110110</t>
+          <t>110100</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.510204081632653</v>
+        <v>0.4235323759133282</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>000111</t>
+          <t>110000</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['000000' '110111']</t>
+          <t>['110110' '001000']</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>-0.7777777777777778</v>
+        <v>0.5238095238095237</v>
       </c>
       <c r="J11" t="n">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>000111</t>
+          <t>110000</t>
         </is>
       </c>
       <c r="L11" t="n">
-        <v>0.6049382716049383</v>
+        <v>0.27437641723356</v>
       </c>
     </row>
   </sheetData>
@@ -1432,402 +1433,402 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-1</v>
+        <v>-0.9682539682539683</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>000000</t>
+          <t>000001</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0.9375157470395565</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>000111</t>
+          <t>001001</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['000111' '000000']</t>
+          <t>['001001' '001000']</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>-0.7777777777777778</v>
+        <v>-0.7142857142857143</v>
       </c>
       <c r="J2" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>000111</t>
+          <t>001001</t>
         </is>
       </c>
       <c r="L2" t="n">
-        <v>0.6049382716049383</v>
+        <v>0.5102040816326531</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-1</v>
+        <v>-0.873015873015873</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>000000</t>
+          <t>000100</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0.762156714537667</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>000000</t>
+          <t>001000</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>['000111' '000000']</t>
+          <t>['001001' '001000']</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>-1</v>
+        <v>-0.746031746031746</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>000000</t>
+          <t>001000</t>
         </is>
       </c>
       <c r="L3" t="n">
-        <v>1</v>
+        <v>0.5565633660871756</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-1</v>
+        <v>-0.8095238095238095</v>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>000000</t>
+          <t>000110</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0.655328798185941</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>000001</t>
+          <t>001000</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['000001' '000001']</t>
+          <t>['001000' '001000']</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>-0.9682539682539683</v>
+        <v>-0.746031746031746</v>
       </c>
       <c r="J4" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>000001</t>
+          <t>001000</t>
         </is>
       </c>
       <c r="L4" t="n">
-        <v>0.9375157470395565</v>
+        <v>0.5565633660871756</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-0.9682539682539683</v>
+        <v>-0.746031746031746</v>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>000001</t>
+          <t>001000</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.9375157470395565</v>
+        <v>0.5565633660871756</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>000001</t>
+          <t>001000</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['000001' '000001']</t>
+          <t>['001000' '001000']</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>-0.9682539682539683</v>
+        <v>-0.746031746031746</v>
       </c>
       <c r="J5" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>000001</t>
+          <t>001000</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>0.9375157470395565</v>
+        <v>0.5565633660871756</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.9682539682539683</v>
+        <v>-0.746031746031746</v>
       </c>
       <c r="B6" t="n">
+        <v>8</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>001000</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.5565633660871756</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>000000</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>['001000' '000110']</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>000000</t>
+        </is>
+      </c>
+      <c r="L6" t="n">
         <v>1</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>000001</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>0.9375157470395565</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>000001</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>['000001' '000000']</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>-0.9682539682539683</v>
-      </c>
-      <c r="J6" t="n">
-        <v>1</v>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>000001</t>
-        </is>
-      </c>
-      <c r="L6" t="n">
-        <v>0.9375157470395565</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-0.8095238095238095</v>
+        <v>-0.746031746031746</v>
       </c>
       <c r="B7" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>000110</t>
+          <t>001000</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.655328798185941</v>
+        <v>0.5565633660871756</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>000000</t>
+          <t>001110</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['000001' '000000']</t>
+          <t>['001000' '000110']</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>-1</v>
+        <v>-0.5555555555555556</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>000000</t>
+          <t>001110</t>
         </is>
       </c>
       <c r="L7" t="n">
-        <v>1</v>
+        <v>0.308641975308642</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-0.7777777777777778</v>
+        <v>-0.746031746031746</v>
       </c>
       <c r="B8" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>000111</t>
+          <t>001000</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.6049382716049383</v>
+        <v>0.5565633660871756</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>000000</t>
+          <t>001000</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['000000' '000111']</t>
+          <t>['001000' '001000']</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>-1</v>
+        <v>-0.746031746031746</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>000000</t>
+          <t>001000</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>1</v>
+        <v>0.5565633660871756</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-0.7777777777777778</v>
+        <v>-0.746031746031746</v>
       </c>
       <c r="B9" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>000111</t>
+          <t>001000</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.6049382716049383</v>
+        <v>0.5565633660871756</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>000111</t>
+          <t>001000</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['000000' '000111']</t>
+          <t>['001000' '001000']</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>-0.7777777777777778</v>
+        <v>-0.746031746031746</v>
       </c>
       <c r="J9" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>000111</t>
+          <t>001000</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>0.6049382716049383</v>
+        <v>0.5565633660871756</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-0.7777777777777778</v>
+        <v>-0.7142857142857143</v>
       </c>
       <c r="B10" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>000111</t>
+          <t>001001</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.6049382716049383</v>
+        <v>0.5102040816326531</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>000111</t>
+          <t>000000</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['110111' '000000']</t>
+          <t>['001000' '000001']</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>-0.7777777777777778</v>
+        <v>-1</v>
       </c>
       <c r="J10" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>000111</t>
+          <t>000000</t>
         </is>
       </c>
       <c r="L10" t="n">
-        <v>0.6049382716049383</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.746031746031746</v>
+        <v>-0.7142857142857143</v>
       </c>
       <c r="B11" t="n">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>110111</t>
+          <t>001001</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.5565633660871756</v>
+        <v>0.5102040816326531</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>110000</t>
+          <t>001001</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['110111' '000000']</t>
+          <t>['001000' '000001']</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>0.5238095238095237</v>
+        <v>-0.7142857142857143</v>
       </c>
       <c r="J11" t="n">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>110000</t>
+          <t>001001</t>
         </is>
       </c>
       <c r="L11" t="n">
-        <v>0.27437641723356</v>
+        <v>0.5102040816326531</v>
       </c>
     </row>
   </sheetData>
@@ -1836,6 +1837,477 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>valor_real</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>valor_normal</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>valor_binario</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>aptitud</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>hijo</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>padres</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>valor_real</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>valor_normal</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>valor_binario</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>aptitud</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>000000</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>000000</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>['000000' '000110']</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>000000</t>
+        </is>
+      </c>
+      <c r="L2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>-1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>000000</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>000110</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>['000000' '000110']</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>-0.8095238095238095</v>
+      </c>
+      <c r="J3" t="n">
+        <v>6</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>000110</t>
+        </is>
+      </c>
+      <c r="L3" t="n">
+        <v>0.655328798185941</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>-0.9682539682539683</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>000001</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.9375157470395565</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>000000</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>['001000' '000000']</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>000000</t>
+        </is>
+      </c>
+      <c r="L4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>-0.873015873015873</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>000100</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.762156714537667</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>001000</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>['001000' '000000']</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>-0.746031746031746</v>
+      </c>
+      <c r="J5" t="n">
+        <v>8</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>001000</t>
+        </is>
+      </c>
+      <c r="L5" t="n">
+        <v>0.5565633660871756</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>-0.8095238095238095</v>
+      </c>
+      <c r="B6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>000110</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.655328798185941</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>000000</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>['001000' '000000']</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>000000</t>
+        </is>
+      </c>
+      <c r="L6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>-0.746031746031746</v>
+      </c>
+      <c r="B7" t="n">
+        <v>8</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>001000</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.5565633660871756</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>001000</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>['001000' '000000']</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>-0.746031746031746</v>
+      </c>
+      <c r="J7" t="n">
+        <v>8</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>001000</t>
+        </is>
+      </c>
+      <c r="L7" t="n">
+        <v>0.5565633660871756</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>-0.746031746031746</v>
+      </c>
+      <c r="B8" t="n">
+        <v>8</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>001000</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.5565633660871756</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>000000</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>['000000' '000001']</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>000000</t>
+        </is>
+      </c>
+      <c r="L8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>-0.746031746031746</v>
+      </c>
+      <c r="B9" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>001000</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.5565633660871756</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>000001</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>['000000' '000001']</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>-0.9682539682539683</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>000001</t>
+        </is>
+      </c>
+      <c r="L9" t="n">
+        <v>0.9375157470395565</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>-0.746031746031746</v>
+      </c>
+      <c r="B10" t="n">
+        <v>8</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>001000</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.5565633660871756</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>001000</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>['000000' '001000']</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>-0.746031746031746</v>
+      </c>
+      <c r="J10" t="n">
+        <v>8</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>001000</t>
+        </is>
+      </c>
+      <c r="L10" t="n">
+        <v>0.5565633660871756</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>-0.746031746031746</v>
+      </c>
+      <c r="B11" t="n">
+        <v>8</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>001000</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.5565633660871756</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>000000</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>['000000' '001000']</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>000000</t>
+        </is>
+      </c>
+      <c r="L11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1969,18 +2441,18 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-0.9682539682539683</v>
+        <v>-1</v>
       </c>
       <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>000000</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
         <v>1</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>000001</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>0.9375157470395565</v>
       </c>
     </row>
     <row r="9">
@@ -2017,18 +2489,18 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>-0.9682539682539683</v>
+        <v>-0.873015873015873</v>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>000001</t>
+          <t>000100</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.9375157470395565</v>
+        <v>0.762156714537667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>